<commit_message>
refactoring and some smooth error handling logic
</commit_message>
<xml_diff>
--- a/kloepfel-task-python-version/handelsregister_result.xlsx
+++ b/kloepfel-task-python-version/handelsregister_result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1631,6 +1631,826 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Marc</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Kloepfel</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>1975-10-03</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Duran</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Sarikaya</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>1978-06-21</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Hans-Christian</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Vastert</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>1988-08-14</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Neuss</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Thanh-Duy</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Tran</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>1979-02-27</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Hamburg</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Hornikel</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>1973-12-22</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Marc</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Kloepfel</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>1975-10-03</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Duran</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Sarikaya</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>1978-06-21</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Hans-Christian</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Vastert</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>1988-08-14</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Neuss</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Thanh-Duy</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tran</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>1979-02-27</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>North Rhine-Westphalia   District court Düsseldorf HRB 55799</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Düsseldorf</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>currently registered</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Kloepfel Consulting GmbH</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Gesellschaft mit beschränkter Haftung</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Cecilienallee</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>6-7</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>40474</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Hamburg</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Hornikel</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>1973-12-22</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Dienstleistungen der allgemeinen Unternehmensberatung und alle damit im Zusammenhang stehenden Geschäfte.</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Ist nur ein Geschäftsführer bestellt, so vertritt er die Gesellschaft allein. Sind mehrere Geschäftsführer bestellt, so wird die Gesellschaft durch zwei Geschäftsführer oder durch einen Geschäftsführer gemeinsam mit einem Prokuristen vertreten. Einem oder mehreren Geschäftsführern kann die Befugnis erteilt werden, die Gesellschaft stets einzeln zu vertreten. Jeder Geschäftsführer kann von den Beschränkungen des § 181 BGB befreit werden.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>